<commit_message>
Update AFOLU test with the last parameters in the yaml file and the last experiment_manager
</commit_message>
<xml_diff>
--- a/tests/AFOLU/t3a_experiments/Experiment_1/_Experiment_Setup.xlsx
+++ b/tests/AFOLU/t3a_experiments/Experiment_1/_Experiment_Setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_GUA\Experiment_AFOLU_3_v3_test5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\tests\AFOLU\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7291DD6-AE6F-4ED9-9F06-BF4D0EC205A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12485348-A43F-4ABF-AF97-CFD5D67913EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30270" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -420,21 +420,21 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>5</v>
       </c>
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -713,7 +713,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FCA711C-FE17-40CB-99DD-D2988BB5DF68}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FCA711C-FE17-40CB-99DD-D2988BB5DF68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1fcbaaf-06d9-47c4-b3a2-beefbc45d784"/>
+    <ds:schemaRef ds:uri="081a93ea-d517-42a5-a2b7-457060aa7471"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>